<commit_message>
updated the git ignore to allow sample data xlsx file
</commit_message>
<xml_diff>
--- a/ex/data.xlsx
+++ b/ex/data.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="0" windowWidth="28300" windowHeight="15720" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="user" sheetId="1" r:id="rId1"/>
+    <sheet name="example" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>email</t>
   </si>
@@ -27,9 +27,6 @@
     <t>gender</t>
   </si>
   <si>
-    <t>Female</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -42,12 +39,6 @@
     <t>facebook.imageurl</t>
   </si>
   <si>
-    <t>name.first</t>
-  </si>
-  <si>
-    <t>name.last</t>
-  </si>
-  <si>
     <t>address,1_location</t>
   </si>
   <si>
@@ -72,22 +63,22 @@
     <t>info@greenpioneersolutions.com</t>
   </si>
   <si>
-    <t>Jason</t>
-  </si>
-  <si>
-    <t>Humphrey</t>
-  </si>
-  <si>
-    <t>Tyler</t>
-  </si>
-  <si>
-    <t>Sorber</t>
-  </si>
-  <si>
     <t>https://graph.facebook.com/1232132121/picture?height=200&amp;width=200&amp;type=square</t>
   </si>
   <si>
     <t>https://graph.facebook.com/1232342143/picture?height=200&amp;width=200&amp;type=square</t>
+  </si>
+  <si>
+    <t>Jason Humphrey</t>
+  </si>
+  <si>
+    <t>Tyler Sorber</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Male</t>
   </si>
 </sst>
 </file>
@@ -492,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -509,91 +500,82 @@
     <col min="48" max="48" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2">
+        <v>1232132121</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2">
-        <v>1232132121</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="E3">
+        <v>1232342143</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="H3" t="s">
         <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3">
-        <v>1232342143</v>
-      </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added content to the read me and updated the mongo uri
</commit_message>
<xml_diff>
--- a/ex/data.xlsx
+++ b/ex/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24426"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="0" windowWidth="28300" windowHeight="15720" tabRatio="500"/>
+    <workbookView xWindow="4900" yWindow="2060" windowWidth="18460" windowHeight="13660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="example" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,6 @@
     <t>email</t>
   </si>
   <si>
-    <t>gender</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -45,9 +42,6 @@
     <t>texas</t>
   </si>
   <si>
-    <t>address,2_location</t>
-  </si>
-  <si>
     <t>florida</t>
   </si>
   <si>
@@ -79,6 +73,12 @@
   </si>
   <si>
     <t>Male</t>
+  </si>
+  <si>
+    <t>gender_</t>
+  </si>
+  <si>
+    <t>addressj,2</t>
   </si>
 </sst>
 </file>
@@ -486,7 +486,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -505,77 +505,77 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
         <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
       </c>
       <c r="E2">
         <v>1232132121</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E3">
         <v>1232342143</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>